<commit_message>
no se estanca maaas
</commit_message>
<xml_diff>
--- a/TP1/tablas/1.xlsx
+++ b/TP1/tablas/1.xlsx
@@ -469,17 +469,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>111010001001111001001000000001</t>
+          <t>111011101110000111011011011111</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.825672412949801</v>
+        <v>0.8707387086646294</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0004760062637729912</v>
+        <v>4.768532367299375e-05</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3795888401714141</v>
+        <v>0.3173840552702083</v>
       </c>
     </row>
     <row r="3">
@@ -491,17 +491,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>111011111010111110000000011010</t>
+          <t>110101010110110110000001101001</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.8766046823019503</v>
+        <v>0.6950593348872544</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1732958563394924</v>
+        <v>0.3187228076815762</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6819056610230266</v>
+        <v>0.552009236047649</v>
       </c>
     </row>
     <row r="4">
@@ -513,17 +513,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>111010001001111001001000000001</t>
+          <t>110101010110110110000001101001</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.825672412949801</v>
+        <v>0.6950593348872544</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6598153960186488</v>
+        <v>0.3187228076815762</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7891955467181526</v>
+        <v>0.6167493181955052</v>
       </c>
     </row>
     <row r="5">
@@ -535,17 +535,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>111010011010111110000000011010</t>
+          <t>110101010110110110000001101001</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.8332662630792799</v>
+        <v>0.6950593348872544</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6598161328539616</v>
+        <v>0.3187228118878417</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7580390756396367</v>
+        <v>0.6447661629039022</v>
       </c>
     </row>
     <row r="6">
@@ -557,17 +557,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>111010001010111110000000011010</t>
+          <t>110101010110110110000001101001</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.8261500047324712</v>
+        <v>0.6950593348872544</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6599517432777053</v>
+        <v>0.3187228118878417</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8049700442729284</v>
+        <v>0.5985504008291642</v>
       </c>
     </row>
     <row r="7">
@@ -579,17 +579,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>111010011010101001000100110111</t>
+          <t>110101010110110110000001101001</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.8331205022195173</v>
+        <v>0.6950593348872544</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8115355546244437</v>
+        <v>0.3193874251293569</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8250988934420848</v>
+        <v>0.580097988249225</v>
       </c>
     </row>
     <row r="8">
@@ -601,17 +601,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>111010011010101110000000011010</t>
+          <t>110101011100011010110100010001</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.8331548368493218</v>
+        <v>0.697330607585406</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8256715853073396</v>
+        <v>0.3204921751343382</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8265601828187951</v>
+        <v>0.5907186045214348</v>
       </c>
     </row>
     <row r="9">
@@ -623,17 +623,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>111010011010101110001000000001</t>
+          <t>110101011100011010110100010001</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.8331556648335329</v>
+        <v>0.697330607585406</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8256715853073396</v>
+        <v>0.3204748987471798</v>
       </c>
       <c r="F9" t="n">
-        <v>0.827486211460522</v>
+        <v>0.5737924374961629</v>
       </c>
     </row>
     <row r="10">
@@ -645,17 +645,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>111010011010101110001000000001</t>
+          <t>110101011100011010110100010001</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.8331556648335329</v>
+        <v>0.697330607585406</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8256715903848995</v>
+        <v>0.3204748987471798</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8287095815878207</v>
+        <v>0.5740195477180339</v>
       </c>
     </row>
     <row r="11">
@@ -667,17 +667,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>111010011010101110001000000001</t>
+          <t>110101011100011010110100010001</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.8331556648335329</v>
+        <v>0.697330607585406</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8256724112572802</v>
+        <v>0.3204921614260828</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8286288375015382</v>
+        <v>0.6219629075920403</v>
       </c>
     </row>
     <row r="12">
@@ -689,17 +689,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>111010011010101110001000000001</t>
+          <t>110101111100011010110100000100</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.8331556648335329</v>
+        <v>0.7104394854017123</v>
       </c>
       <c r="E12" t="n">
-        <v>0.8256724112572802</v>
+        <v>0.6973305873648619</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8278805187913104</v>
+        <v>0.6986414791906014</v>
       </c>
     </row>
     <row r="13">
@@ -711,17 +711,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>111010011011111001001000000000</t>
+          <t>110101011100011010110100010001</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.8336780382375061</v>
+        <v>0.697330607585406</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8251525524160778</v>
+        <v>0.6973305873648619</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8264210349540099</v>
+        <v>0.6973305954530795</v>
       </c>
     </row>
     <row r="14">
@@ -733,17 +733,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>111010011011111001001000110111</t>
+          <t>110101011100011011110100000100</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.8336781317763521</v>
+        <v>0.6973369584062109</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8256724112572802</v>
+        <v>0.697330581143156</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8264730212216541</v>
+        <v>0.697331227890935</v>
       </c>
     </row>
     <row r="15">
@@ -755,17 +755,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>111010001001111001001000110111</t>
+          <t>110101011100011011110100000101</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.8256725043459264</v>
+        <v>0.6973369599616445</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8256724112572802</v>
+        <v>0.6973289946090721</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8256724583093595</v>
+        <v>0.6973317057194917</v>
       </c>
     </row>
     <row r="16">
@@ -777,17 +777,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>111010001001111001001000110111</t>
+          <t>110101011100011011110100000100</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.8256725043459264</v>
+        <v>0.6973369584062109</v>
       </c>
       <c r="E16" t="n">
-        <v>0.8256724112572802</v>
+        <v>0.6973289946090721</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8256724583093595</v>
+        <v>0.6973315464439119</v>
       </c>
     </row>
     <row r="17">
@@ -799,17 +799,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>111010001001111001001001110111</t>
+          <t>110101011100011010110100010001</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.825672612667267</v>
+        <v>0.697330607585406</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8221267525877607</v>
+        <v>0.6973289946090721</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8253178846568124</v>
+        <v>0.6973304321333917</v>
       </c>
     </row>
     <row r="18">
@@ -821,17 +821,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>111010001001111001001001110111</t>
+          <t>110101011100011010110100010000</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.825672612667267</v>
+        <v>0.6973306060299795</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8221267525877607</v>
+        <v>0.6973289946090721</v>
       </c>
       <c r="F18" t="n">
-        <v>0.8249411198232112</v>
+        <v>0.6973302706802156</v>
       </c>
     </row>
     <row r="19">
@@ -843,17 +843,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>111010001101111001001000000000</t>
+          <t>110101011100011010110100010000</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.8274481016149946</v>
+        <v>0.6973306060299795</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8221267525877607</v>
+        <v>0.6973305873648619</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8251187266018578</v>
+        <v>0.6973305892313736</v>
       </c>
     </row>
     <row r="20">
@@ -865,17 +865,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>111010001001111001001001110111</t>
+          <t>110101111100011010110100000100</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.825672612667267</v>
+        <v>0.7104394854017123</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8221267525877607</v>
+        <v>0.6973305873648619</v>
       </c>
       <c r="F20" t="n">
-        <v>0.8246087346433196</v>
+        <v>0.6986414827680821</v>
       </c>
     </row>
     <row r="21">
@@ -887,17 +887,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>111010001001111001001001110111</t>
+          <t>110101111100011010110100010000</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.825672612667267</v>
+        <v>0.710439504241453</v>
       </c>
       <c r="E21" t="n">
-        <v>0.8221267525877607</v>
+        <v>0.6973305873648619</v>
       </c>
       <c r="F21" t="n">
-        <v>0.8242541689448922</v>
+        <v>0.6986414829410872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>